<commit_message>
Update Excel with new data [auto]
</commit_message>
<xml_diff>
--- a/bconomy.xlsx
+++ b/bconomy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>2025-07-07T14:38</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2025-07-07T14:43</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +469,9 @@
       <c r="C2" t="n">
         <v>100</v>
       </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,6 +487,9 @@
       <c r="C3" t="n">
         <v>600</v>
       </c>
+      <c r="D3" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,6 +505,9 @@
       <c r="C4" t="n">
         <v>200</v>
       </c>
+      <c r="D4" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -509,6 +523,9 @@
       <c r="C5" t="n">
         <v>800</v>
       </c>
+      <c r="D5" t="n">
+        <v>800</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -524,6 +541,9 @@
       <c r="C6" t="n">
         <v>300</v>
       </c>
+      <c r="D6" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -539,6 +559,9 @@
       <c r="C7" t="n">
         <v>14900</v>
       </c>
+      <c r="D7" t="n">
+        <v>14900</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -554,6 +577,9 @@
       <c r="C8" t="n">
         <v>1200</v>
       </c>
+      <c r="D8" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -569,6 +595,9 @@
       <c r="C9" t="n">
         <v>1100</v>
       </c>
+      <c r="D9" t="n">
+        <v>1100</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -584,6 +613,9 @@
       <c r="C10" t="n">
         <v>1700</v>
       </c>
+      <c r="D10" t="n">
+        <v>1700</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -599,6 +631,9 @@
       <c r="C11" t="n">
         <v>8800</v>
       </c>
+      <c r="D11" t="n">
+        <v>8800</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -614,6 +649,9 @@
       <c r="C12" t="n">
         <v>12700</v>
       </c>
+      <c r="D12" t="n">
+        <v>12700</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -629,6 +667,9 @@
       <c r="C13" t="n">
         <v>59900</v>
       </c>
+      <c r="D13" t="n">
+        <v>59900</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -644,6 +685,9 @@
       <c r="C14" t="n">
         <v>689900</v>
       </c>
+      <c r="D14" t="n">
+        <v>689900</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -659,6 +703,9 @@
       <c r="C15" t="n">
         <v>255000</v>
       </c>
+      <c r="D15" t="n">
+        <v>255000</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -674,6 +721,9 @@
       <c r="C16" t="n">
         <v>4600000</v>
       </c>
+      <c r="D16" t="n">
+        <v>4600000</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -689,6 +739,9 @@
       <c r="C17" t="n">
         <v>57900</v>
       </c>
+      <c r="D17" t="n">
+        <v>57900</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -704,6 +757,9 @@
       <c r="C18" t="n">
         <v>250000</v>
       </c>
+      <c r="D18" t="n">
+        <v>250000</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -719,6 +775,9 @@
       <c r="C19" t="n">
         <v>24900</v>
       </c>
+      <c r="D19" t="n">
+        <v>24900</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -734,6 +793,9 @@
       <c r="C20" t="n">
         <v>2000000</v>
       </c>
+      <c r="D20" t="n">
+        <v>2000000</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -749,6 +811,9 @@
       <c r="C21" t="n">
         <v>140000</v>
       </c>
+      <c r="D21" t="n">
+        <v>140000</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -764,6 +829,9 @@
       <c r="C22" t="n">
         <v>14999000</v>
       </c>
+      <c r="D22" t="n">
+        <v>14999000</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -779,6 +847,9 @@
       <c r="C23" t="n">
         <v>195000</v>
       </c>
+      <c r="D23" t="n">
+        <v>195000</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -794,6 +865,9 @@
       <c r="C24" t="n">
         <v>2800</v>
       </c>
+      <c r="D24" t="n">
+        <v>2800</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -809,6 +883,9 @@
       <c r="C25" t="n">
         <v>2499000</v>
       </c>
+      <c r="D25" t="n">
+        <v>2499000</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -824,6 +901,9 @@
       <c r="C26" t="n">
         <v>144600</v>
       </c>
+      <c r="D26" t="n">
+        <v>144600</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -839,6 +919,9 @@
       <c r="C27" t="n">
         <v>4469800</v>
       </c>
+      <c r="D27" t="n">
+        <v>4469800</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -854,6 +937,9 @@
       <c r="C28" t="n">
         <v>540000</v>
       </c>
+      <c r="D28" t="n">
+        <v>540000</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -869,6 +955,9 @@
       <c r="C29" t="n">
         <v>999999900</v>
       </c>
+      <c r="D29" t="n">
+        <v>999999900</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -884,6 +973,9 @@
       <c r="C30" t="n">
         <v>500000</v>
       </c>
+      <c r="D30" t="n">
+        <v>500000</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -899,6 +991,9 @@
       <c r="C31" t="n">
         <v>2000000</v>
       </c>
+      <c r="D31" t="n">
+        <v>2000000</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -914,6 +1009,9 @@
       <c r="C32" t="n">
         <v>599900</v>
       </c>
+      <c r="D32" t="n">
+        <v>599900</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -929,6 +1027,9 @@
       <c r="C33" t="n">
         <v>15900</v>
       </c>
+      <c r="D33" t="n">
+        <v>15900</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -944,6 +1045,9 @@
       <c r="C34" t="n">
         <v>44900</v>
       </c>
+      <c r="D34" t="n">
+        <v>44900</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -959,6 +1063,9 @@
       <c r="C35" t="n">
         <v>44700</v>
       </c>
+      <c r="D35" t="n">
+        <v>44700</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -974,6 +1081,9 @@
       <c r="C36" t="n">
         <v>35000</v>
       </c>
+      <c r="D36" t="n">
+        <v>35000</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -989,6 +1099,9 @@
       <c r="C37" t="n">
         <v>25000000</v>
       </c>
+      <c r="D37" t="n">
+        <v>25000000</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1004,6 +1117,9 @@
       <c r="C38" t="n">
         <v>25000000</v>
       </c>
+      <c r="D38" t="n">
+        <v>25000000</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1019,6 +1135,9 @@
       <c r="C39" t="n">
         <v>1500000</v>
       </c>
+      <c r="D39" t="n">
+        <v>1500000</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1034,6 +1153,9 @@
       <c r="C40" t="n">
         <v>1400000000</v>
       </c>
+      <c r="D40" t="n">
+        <v>1400000000</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1047,6 +1169,7 @@
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1062,6 +1185,9 @@
       <c r="C42" t="n">
         <v>439000000</v>
       </c>
+      <c r="D42" t="n">
+        <v>439000000</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1077,6 +1203,9 @@
       <c r="C43" t="n">
         <v>800000000</v>
       </c>
+      <c r="D43" t="n">
+        <v>800000000</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1092,6 +1221,9 @@
       <c r="C44" t="n">
         <v>99000000</v>
       </c>
+      <c r="D44" t="n">
+        <v>99000000</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1107,6 +1239,9 @@
       <c r="C45" t="n">
         <v>274500</v>
       </c>
+      <c r="D45" t="n">
+        <v>274500</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1122,6 +1257,9 @@
       <c r="C46" t="n">
         <v>399998000</v>
       </c>
+      <c r="D46" t="n">
+        <v>399998000</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1137,6 +1275,9 @@
       <c r="C47" t="n">
         <v>200000</v>
       </c>
+      <c r="D47" t="n">
+        <v>200000</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1152,6 +1293,9 @@
       <c r="C48" t="n">
         <v>100</v>
       </c>
+      <c r="D48" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1167,6 +1311,9 @@
       <c r="C49" t="n">
         <v>200</v>
       </c>
+      <c r="D49" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1182,6 +1329,9 @@
       <c r="C50" t="n">
         <v>200</v>
       </c>
+      <c r="D50" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1197,6 +1347,9 @@
       <c r="C51" t="n">
         <v>400</v>
       </c>
+      <c r="D51" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1212,6 +1365,9 @@
       <c r="C52" t="n">
         <v>1200</v>
       </c>
+      <c r="D52" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1227,6 +1383,9 @@
       <c r="C53" t="n">
         <v>600</v>
       </c>
+      <c r="D53" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1242,6 +1401,9 @@
       <c r="C54" t="n">
         <v>1800</v>
       </c>
+      <c r="D54" t="n">
+        <v>1800</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1257,6 +1419,9 @@
       <c r="C55" t="n">
         <v>13900</v>
       </c>
+      <c r="D55" t="n">
+        <v>13900</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1272,6 +1437,9 @@
       <c r="C56" t="n">
         <v>6600</v>
       </c>
+      <c r="D56" t="n">
+        <v>6600</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1287,6 +1455,9 @@
       <c r="C57" t="n">
         <v>100000</v>
       </c>
+      <c r="D57" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1302,6 +1473,9 @@
       <c r="C58" t="n">
         <v>12500</v>
       </c>
+      <c r="D58" t="n">
+        <v>12500</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1317,6 +1491,9 @@
       <c r="C59" t="n">
         <v>58500</v>
       </c>
+      <c r="D59" t="n">
+        <v>58500</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1332,6 +1509,9 @@
       <c r="C60" t="n">
         <v>52700</v>
       </c>
+      <c r="D60" t="n">
+        <v>52700</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1347,6 +1527,9 @@
       <c r="C61" t="n">
         <v>239900</v>
       </c>
+      <c r="D61" t="n">
+        <v>239900</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1362,6 +1545,9 @@
       <c r="C62" t="n">
         <v>598900</v>
       </c>
+      <c r="D62" t="n">
+        <v>598900</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1377,6 +1563,9 @@
       <c r="C63" t="n">
         <v>2400000</v>
       </c>
+      <c r="D63" t="n">
+        <v>2400000</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1392,6 +1581,9 @@
       <c r="C64" t="n">
         <v>39000000</v>
       </c>
+      <c r="D64" t="n">
+        <v>39000000</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1407,6 +1599,9 @@
       <c r="C65" t="n">
         <v>3900000</v>
       </c>
+      <c r="D65" t="n">
+        <v>3900000</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1422,6 +1617,9 @@
       <c r="C66" t="n">
         <v>10000000</v>
       </c>
+      <c r="D66" t="n">
+        <v>10000000</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1437,6 +1635,9 @@
       <c r="C67" t="n">
         <v>2500000</v>
       </c>
+      <c r="D67" t="n">
+        <v>2500000</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1452,6 +1653,9 @@
       <c r="C68" t="n">
         <v>100</v>
       </c>
+      <c r="D68" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1467,6 +1671,9 @@
       <c r="C69" t="n">
         <v>200</v>
       </c>
+      <c r="D69" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1482,6 +1689,9 @@
       <c r="C70" t="n">
         <v>1100</v>
       </c>
+      <c r="D70" t="n">
+        <v>1100</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1497,6 +1707,9 @@
       <c r="C71" t="n">
         <v>700</v>
       </c>
+      <c r="D71" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1512,6 +1725,9 @@
       <c r="C72" t="n">
         <v>600</v>
       </c>
+      <c r="D72" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1527,6 +1743,9 @@
       <c r="C73" t="n">
         <v>1300</v>
       </c>
+      <c r="D73" t="n">
+        <v>1300</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1542,6 +1761,9 @@
       <c r="C74" t="n">
         <v>2900</v>
       </c>
+      <c r="D74" t="n">
+        <v>2900</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1557,6 +1779,9 @@
       <c r="C75" t="n">
         <v>1700</v>
       </c>
+      <c r="D75" t="n">
+        <v>1700</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1572,6 +1797,9 @@
       <c r="C76" t="n">
         <v>14900</v>
       </c>
+      <c r="D76" t="n">
+        <v>14900</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1587,6 +1815,9 @@
       <c r="C77" t="n">
         <v>94900</v>
       </c>
+      <c r="D77" t="n">
+        <v>94900</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1602,6 +1833,9 @@
       <c r="C78" t="n">
         <v>937400</v>
       </c>
+      <c r="D78" t="n">
+        <v>937400</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1617,6 +1851,9 @@
       <c r="C79" t="n">
         <v>24000000</v>
       </c>
+      <c r="D79" t="n">
+        <v>24000000</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1632,6 +1869,9 @@
       <c r="C80" t="n">
         <v>75000000</v>
       </c>
+      <c r="D80" t="n">
+        <v>75000000</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1647,6 +1887,9 @@
       <c r="C81" t="n">
         <v>23599999000</v>
       </c>
+      <c r="D81" t="n">
+        <v>23599999000</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1662,6 +1905,9 @@
       <c r="C82" t="n">
         <v>740000000</v>
       </c>
+      <c r="D82" t="n">
+        <v>740000000</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1677,6 +1923,9 @@
       <c r="C83" t="n">
         <v>5480000</v>
       </c>
+      <c r="D83" t="n">
+        <v>5480000</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1692,6 +1941,9 @@
       <c r="C84" t="n">
         <v>1200</v>
       </c>
+      <c r="D84" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1707,6 +1959,9 @@
       <c r="C85" t="n">
         <v>295000</v>
       </c>
+      <c r="D85" t="n">
+        <v>295000</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1722,6 +1977,9 @@
       <c r="C86" t="n">
         <v>3750000</v>
       </c>
+      <c r="D86" t="n">
+        <v>3750000</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1737,6 +1995,9 @@
       <c r="C87" t="n">
         <v>19990000000</v>
       </c>
+      <c r="D87" t="n">
+        <v>19990000000</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1752,6 +2013,9 @@
       <c r="C88" t="n">
         <v>250000000000</v>
       </c>
+      <c r="D88" t="n">
+        <v>250000000000</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1767,6 +2031,9 @@
       <c r="C89" t="n">
         <v>1000000000</v>
       </c>
+      <c r="D89" t="n">
+        <v>1000000000</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1782,6 +2049,9 @@
       <c r="C90" t="n">
         <v>1700000000</v>
       </c>
+      <c r="D90" t="n">
+        <v>1700000000</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1797,6 +2067,9 @@
       <c r="C91" t="n">
         <v>20220201900</v>
       </c>
+      <c r="D91" t="n">
+        <v>20220201900</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1812,6 +2085,9 @@
       <c r="C92" t="n">
         <v>2100000000</v>
       </c>
+      <c r="D92" t="n">
+        <v>2100000000</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1827,6 +2103,9 @@
       <c r="C93" t="n">
         <v>970000000000</v>
       </c>
+      <c r="D93" t="n">
+        <v>970000000000</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1842,6 +2121,9 @@
       <c r="C94" t="n">
         <v>600</v>
       </c>
+      <c r="D94" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1857,6 +2139,9 @@
       <c r="C95" t="n">
         <v>200</v>
       </c>
+      <c r="D95" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1872,6 +2157,9 @@
       <c r="C96" t="n">
         <v>300</v>
       </c>
+      <c r="D96" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1887,6 +2175,9 @@
       <c r="C97" t="n">
         <v>400</v>
       </c>
+      <c r="D97" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1902,6 +2193,9 @@
       <c r="C98" t="n">
         <v>500</v>
       </c>
+      <c r="D98" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1917,6 +2211,9 @@
       <c r="C99" t="n">
         <v>600</v>
       </c>
+      <c r="D99" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1932,6 +2229,9 @@
       <c r="C100" t="n">
         <v>1000</v>
       </c>
+      <c r="D100" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1947,6 +2247,9 @@
       <c r="C101" t="n">
         <v>93200</v>
       </c>
+      <c r="D101" t="n">
+        <v>93200</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1962,6 +2265,9 @@
       <c r="C102" t="n">
         <v>52400</v>
       </c>
+      <c r="D102" t="n">
+        <v>52400</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1977,6 +2283,9 @@
       <c r="C103" t="n">
         <v>526100</v>
       </c>
+      <c r="D103" t="n">
+        <v>526100</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1992,6 +2301,9 @@
       <c r="C104" t="n">
         <v>549700</v>
       </c>
+      <c r="D104" t="n">
+        <v>549800</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2007,6 +2319,9 @@
       <c r="C105" t="n">
         <v>10800</v>
       </c>
+      <c r="D105" t="n">
+        <v>10800</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2022,6 +2337,9 @@
       <c r="C106" t="n">
         <v>4000</v>
       </c>
+      <c r="D106" t="n">
+        <v>4000</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2037,6 +2355,9 @@
       <c r="C107" t="n">
         <v>11900</v>
       </c>
+      <c r="D107" t="n">
+        <v>11900</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2052,6 +2373,9 @@
       <c r="C108" t="n">
         <v>50000</v>
       </c>
+      <c r="D108" t="n">
+        <v>50000</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2067,6 +2391,9 @@
       <c r="C109" t="n">
         <v>2500000</v>
       </c>
+      <c r="D109" t="n">
+        <v>2500000</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2082,6 +2409,9 @@
       <c r="C110" t="n">
         <v>550000000</v>
       </c>
+      <c r="D110" t="n">
+        <v>550000000</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2097,6 +2427,9 @@
       <c r="C111" t="n">
         <v>20000000</v>
       </c>
+      <c r="D111" t="n">
+        <v>20000000</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2112,6 +2445,9 @@
       <c r="C112" t="n">
         <v>1149999000</v>
       </c>
+      <c r="D112" t="n">
+        <v>1149999000</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2127,6 +2463,9 @@
       <c r="C113" t="n">
         <v>17998000000</v>
       </c>
+      <c r="D113" t="n">
+        <v>17998000000</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2142,6 +2481,9 @@
       <c r="C114" t="n">
         <v>114000000000</v>
       </c>
+      <c r="D114" t="n">
+        <v>114000000000</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2157,6 +2499,9 @@
       <c r="C115" t="n">
         <v>60000000000</v>
       </c>
+      <c r="D115" t="n">
+        <v>60000000000</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2172,6 +2517,9 @@
       <c r="C116" t="n">
         <v>49900</v>
       </c>
+      <c r="D116" t="n">
+        <v>49900</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2187,6 +2535,9 @@
       <c r="C117" t="n">
         <v>298000000</v>
       </c>
+      <c r="D117" t="n">
+        <v>298000000</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2202,6 +2553,9 @@
       <c r="C118" t="n">
         <v>300000000</v>
       </c>
+      <c r="D118" t="n">
+        <v>300000000</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2217,6 +2571,9 @@
       <c r="C119" t="n">
         <v>5000000</v>
       </c>
+      <c r="D119" t="n">
+        <v>5000000</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2232,6 +2589,9 @@
       <c r="C120" t="n">
         <v>939999999900</v>
       </c>
+      <c r="D120" t="n">
+        <v>939999999900</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2247,6 +2607,9 @@
       <c r="C121" t="n">
         <v>11900</v>
       </c>
+      <c r="D121" t="n">
+        <v>11900</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2262,6 +2625,9 @@
       <c r="C122" t="n">
         <v>100000</v>
       </c>
+      <c r="D122" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2277,6 +2643,9 @@
       <c r="C123" t="n">
         <v>95000</v>
       </c>
+      <c r="D123" t="n">
+        <v>95000</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2292,6 +2661,9 @@
       <c r="C124" t="n">
         <v>2222200</v>
       </c>
+      <c r="D124" t="n">
+        <v>2222200</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2307,6 +2679,9 @@
       <c r="C125" t="n">
         <v>848900</v>
       </c>
+      <c r="D125" t="n">
+        <v>848900</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2322,6 +2697,9 @@
       <c r="C126" t="n">
         <v>9000000</v>
       </c>
+      <c r="D126" t="n">
+        <v>9000000</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2337,6 +2715,9 @@
       <c r="C127" t="n">
         <v>44999900</v>
       </c>
+      <c r="D127" t="n">
+        <v>44999900</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2352,6 +2733,9 @@
       <c r="C128" t="n">
         <v>950000000000</v>
       </c>
+      <c r="D128" t="n">
+        <v>950000000000</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2367,6 +2751,9 @@
       <c r="C129" t="n">
         <v>59500</v>
       </c>
+      <c r="D129" t="n">
+        <v>59500</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2382,6 +2769,9 @@
       <c r="C130" t="n">
         <v>59400</v>
       </c>
+      <c r="D130" t="n">
+        <v>59400</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2397,6 +2787,9 @@
       <c r="C131" t="n">
         <v>16500000</v>
       </c>
+      <c r="D131" t="n">
+        <v>16500000</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2412,6 +2805,9 @@
       <c r="C132" t="n">
         <v>29999900</v>
       </c>
+      <c r="D132" t="n">
+        <v>29999900</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2427,6 +2823,9 @@
       <c r="C133" t="n">
         <v>4689900</v>
       </c>
+      <c r="D133" t="n">
+        <v>4689900</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2442,6 +2841,9 @@
       <c r="C134" t="n">
         <v>68500000</v>
       </c>
+      <c r="D134" t="n">
+        <v>68500000</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2457,6 +2859,9 @@
       <c r="C135" t="n">
         <v>399997000</v>
       </c>
+      <c r="D135" t="n">
+        <v>399997000</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2472,6 +2877,9 @@
       <c r="C136" t="n">
         <v>395000000</v>
       </c>
+      <c r="D136" t="n">
+        <v>395000000</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2487,6 +2895,9 @@
       <c r="C137" t="n">
         <v>99999000</v>
       </c>
+      <c r="D137" t="n">
+        <v>99999000</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2502,6 +2913,9 @@
       <c r="C138" t="n">
         <v>83889000</v>
       </c>
+      <c r="D138" t="n">
+        <v>83889000</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2517,6 +2931,9 @@
       <c r="C139" t="n">
         <v>3200000000</v>
       </c>
+      <c r="D139" t="n">
+        <v>3200000000</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2532,6 +2949,9 @@
       <c r="C140" t="n">
         <v>12500000000</v>
       </c>
+      <c r="D140" t="n">
+        <v>12500000000</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2547,6 +2967,9 @@
       <c r="C141" t="n">
         <v>44950000000</v>
       </c>
+      <c r="D141" t="n">
+        <v>44950000000</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2562,6 +2985,9 @@
       <c r="C142" t="n">
         <v>10000000000</v>
       </c>
+      <c r="D142" t="n">
+        <v>10000000000</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2577,6 +3003,9 @@
       <c r="C143" t="n">
         <v>147990000</v>
       </c>
+      <c r="D143" t="n">
+        <v>147990000</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2592,6 +3021,9 @@
       <c r="C144" t="n">
         <v>90000000000</v>
       </c>
+      <c r="D144" t="n">
+        <v>90000000000</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2607,6 +3039,9 @@
       <c r="C145" t="n">
         <v>75000000000</v>
       </c>
+      <c r="D145" t="n">
+        <v>75000000000</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2622,6 +3057,9 @@
       <c r="C146" t="n">
         <v>80000000000</v>
       </c>
+      <c r="D146" t="n">
+        <v>80000000000</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2637,6 +3075,9 @@
       <c r="C147" t="n">
         <v>80000000000</v>
       </c>
+      <c r="D147" t="n">
+        <v>80000000000</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2652,6 +3093,9 @@
       <c r="C148" t="n">
         <v>8000000000</v>
       </c>
+      <c r="D148" t="n">
+        <v>8000000000</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2667,6 +3111,9 @@
       <c r="C149" t="n">
         <v>6000000000</v>
       </c>
+      <c r="D149" t="n">
+        <v>6000000000</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2682,6 +3129,9 @@
       <c r="C150" t="n">
         <v>15500000000</v>
       </c>
+      <c r="D150" t="n">
+        <v>15500000000</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2697,6 +3147,9 @@
       <c r="C151" t="n">
         <v>30000000000</v>
       </c>
+      <c r="D151" t="n">
+        <v>30000000000</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2712,6 +3165,9 @@
       <c r="C152" t="n">
         <v>60000000000</v>
       </c>
+      <c r="D152" t="n">
+        <v>60000000000</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2727,6 +3183,9 @@
       <c r="C153" t="n">
         <v>2780000</v>
       </c>
+      <c r="D153" t="n">
+        <v>2780000</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2742,6 +3201,9 @@
       <c r="C154" t="n">
         <v>1350000000</v>
       </c>
+      <c r="D154" t="n">
+        <v>1300000000</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2757,6 +3219,9 @@
       <c r="C155" t="n">
         <v>3900000000</v>
       </c>
+      <c r="D155" t="n">
+        <v>3900000000</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2772,6 +3237,9 @@
       <c r="C156" t="n">
         <v>1000000000</v>
       </c>
+      <c r="D156" t="n">
+        <v>1300000000</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2787,6 +3255,9 @@
       <c r="C157" t="n">
         <v>850000000000</v>
       </c>
+      <c r="D157" t="n">
+        <v>850000000000</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2802,6 +3273,9 @@
       <c r="C158" t="n">
         <v>492000000</v>
       </c>
+      <c r="D158" t="n">
+        <v>492000000</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2817,6 +3291,9 @@
       <c r="C159" t="n">
         <v>12500000000</v>
       </c>
+      <c r="D159" t="n">
+        <v>12500000000</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2832,6 +3309,9 @@
       <c r="C160" t="n">
         <v>300000000000</v>
       </c>
+      <c r="D160" t="n">
+        <v>300000000000</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2847,6 +3327,9 @@
       <c r="C161" t="n">
         <v>900000000000</v>
       </c>
+      <c r="D161" t="n">
+        <v>900000000000</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2862,6 +3345,9 @@
       <c r="C162" t="n">
         <v>955555555500</v>
       </c>
+      <c r="D162" t="n">
+        <v>955555555500</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2877,6 +3363,9 @@
       <c r="C163" t="n">
         <v>1000000000000</v>
       </c>
+      <c r="D163" t="n">
+        <v>1000000000000</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2892,6 +3381,9 @@
       <c r="C164" t="n">
         <v>880000000000</v>
       </c>
+      <c r="D164" t="n">
+        <v>880000000000</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2907,6 +3399,9 @@
       <c r="C165" t="n">
         <v>33900000000</v>
       </c>
+      <c r="D165" t="n">
+        <v>33900000000</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2920,6 +3415,9 @@
         </is>
       </c>
       <c r="C166" t="n">
+        <v>15000000000</v>
+      </c>
+      <c r="D166" t="n">
         <v>15000000000</v>
       </c>
     </row>

</xml_diff>